<commit_message>
SPO - gabby jay done
</commit_message>
<xml_diff>
--- a/SuperPunchout/FrameCompare.xlsx
+++ b/SuperPunchout/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperPunchout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870F66D3-7AF0-48A9-AD13-200CD365C766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD8549-CDDD-4B85-B84A-F75D7513B13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="4485" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Place</t>
   </si>
@@ -118,6 +118,39 @@
   </si>
   <si>
     <t>Logo disappears</t>
+  </si>
+  <si>
+    <t>Title screen appears</t>
+  </si>
+  <si>
+    <t>Title screen disappears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabby jay intro </t>
+  </si>
+  <si>
+    <t>Gabby jay start</t>
+  </si>
+  <si>
+    <t>1st hit</t>
+  </si>
+  <si>
+    <t>stun punch</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>10 count</t>
+  </si>
+  <si>
+    <t>black screen</t>
+  </si>
+  <si>
+    <t>black screen (records)</t>
+  </si>
+  <si>
+    <t>Bear Hugger appears</t>
   </si>
 </sst>
 </file>
@@ -127,12 +160,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -262,33 +302,34 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
@@ -2213,11 +2254,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2245,215 +2286,307 @@
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>190</v>
+      </c>
       <c r="C2" s="2">
         <v>190</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D9" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D19" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2">
+        <v>259</v>
+      </c>
+      <c r="C3" s="2">
+        <v>259</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>396</v>
+      </c>
+      <c r="C4" s="2">
+        <v>396</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2">
+        <v>653</v>
+      </c>
+      <c r="C5" s="2">
+        <v>653</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2">
+        <v>820</v>
+      </c>
+      <c r="C6" s="2">
+        <v>820</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.03</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.03</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.26</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6.26</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2328</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2328</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3019</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3019</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3145</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3145</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3421</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3421</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="str">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4">
+        <v>57254</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" ref="D20" si="1">IF(C20&lt;&gt;"",IF(B20&lt;&gt;"",C20-B20,"-"), "-")</f>
         <v>-</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4">
-        <v>57254</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" ref="D10" si="1">IF(C10&lt;&gt;"",IF(B10&lt;&gt;"",C10-B10,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="12" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2523,89 +2656,109 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
     </row>
@@ -3076,6 +3229,46 @@
     <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
+    </row>
+    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+    </row>
+    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+    </row>
+    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+    </row>
+    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="C185" s="4"/>
+    </row>
+    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="C186" s="4"/>
+    </row>
+    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+      <c r="C187" s="4"/>
+    </row>
+    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+    </row>
+    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="4"/>
+      <c r="C189" s="4"/>
+    </row>
+    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="4"/>
+      <c r="C190" s="4"/>
+    </row>
+    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="4"/>
+      <c r="C191" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SPO - up to Mad Clown
</commit_message>
<xml_diff>
--- a/SuperPunchout/FrameCompare.xlsx
+++ b/SuperPunchout/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperPunchout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD8549-CDDD-4B85-B84A-F75D7513B13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D24D7FA-5BCF-4AC3-ABA6-65DB877AFE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="4485" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="5115" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
   <si>
     <t>Place</t>
   </si>
@@ -151,6 +151,141 @@
   </si>
   <si>
     <t>Bear Hugger appears</t>
+  </si>
+  <si>
+    <t>2nd hit</t>
+  </si>
+  <si>
+    <t>3rd hit</t>
+  </si>
+  <si>
+    <t>phase 1</t>
+  </si>
+  <si>
+    <t>Piston Hurricane intro</t>
+  </si>
+  <si>
+    <t>Piston Hurricane</t>
+  </si>
+  <si>
+    <t>4th hit (gut)</t>
+  </si>
+  <si>
+    <t>5th hit (face)</t>
+  </si>
+  <si>
+    <t>6th hit (gut)</t>
+  </si>
+  <si>
+    <t>7th hit (face)</t>
+  </si>
+  <si>
+    <t>Bald bull</t>
+  </si>
+  <si>
+    <t>1st hit (r gut)</t>
+  </si>
+  <si>
+    <t>2nd hit (r gut)</t>
+  </si>
+  <si>
+    <t>3rd hit (r gut stun)</t>
+  </si>
+  <si>
+    <t>final hit</t>
+  </si>
+  <si>
+    <t>2nd to last hit</t>
+  </si>
+  <si>
+    <t>phase 3 start (transparent)</t>
+  </si>
+  <si>
+    <t>start charge</t>
+  </si>
+  <si>
+    <t>black screen (circuit records)</t>
+  </si>
+  <si>
+    <t>black screen (circuit)</t>
+  </si>
+  <si>
+    <t>black screen (pick major)</t>
+  </si>
+  <si>
+    <t>Bob Charlie</t>
+  </si>
+  <si>
+    <t>4th hit (right face)</t>
+  </si>
+  <si>
+    <t>04"86</t>
+  </si>
+  <si>
+    <t>Dragon Chan</t>
+  </si>
+  <si>
+    <t>7"30</t>
+  </si>
+  <si>
+    <t>Masked Muscle</t>
+  </si>
+  <si>
+    <t>1st hit (gut)</t>
+  </si>
+  <si>
+    <t>3rd hit (face)</t>
+  </si>
+  <si>
+    <t>5th hit (stun)</t>
+  </si>
+  <si>
+    <t>4th hit (face</t>
+  </si>
+  <si>
+    <t>6th hit (late)</t>
+  </si>
+  <si>
+    <t>7th hit (gut)</t>
+  </si>
+  <si>
+    <t>Mr. Sandman</t>
+  </si>
+  <si>
+    <t>1st hit (face)</t>
+  </si>
+  <si>
+    <t>5th hit (gut)</t>
+  </si>
+  <si>
+    <t>phase 3 1st hit (super)</t>
+  </si>
+  <si>
+    <t>black screen (cicuit pick)</t>
+  </si>
+  <si>
+    <t>Aran Ryan</t>
+  </si>
+  <si>
+    <t>3rd hit (r face)</t>
+  </si>
+  <si>
+    <t>5th hit (delay)</t>
+  </si>
+  <si>
+    <t>1st hit (super gut)</t>
+  </si>
+  <si>
+    <t>Heiki Kagero</t>
+  </si>
+  <si>
+    <t>6th hit (stun)</t>
+  </si>
+  <si>
+    <t>dizzy</t>
+  </si>
+  <si>
+    <t>Mad Clown</t>
   </si>
 </sst>
 </file>
@@ -313,7 +448,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -331,6 +466,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -2254,11 +2390,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2293,7 +2429,7 @@
         <v>190</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D19" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D123" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -2435,16 +2571,16 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="6">
         <v>3145</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="6">
         <v>3145</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2465,684 +2601,1681 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="str">
+      <c r="A16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.22</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.22</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6.92</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6.92</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2">
+        <v>10.32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>10.32</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2">
+        <v>12.86</v>
+      </c>
+      <c r="C19" s="16">
+        <v>12.86</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2">
+        <v>12.92</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12.92</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2">
+        <v>6090</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6090</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2">
+        <v>6781</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6781</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="6">
+        <v>6907</v>
+      </c>
+      <c r="C23" s="6">
+        <v>6907</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2">
+        <v>6996</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6996</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7173</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7173</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4.37</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4.37</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2">
+        <v>5.49</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5.49</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2">
+        <v>9766</v>
+      </c>
+      <c r="C34" s="2">
+        <v>9766</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="6">
+        <v>9892</v>
+      </c>
+      <c r="C35" s="6">
+        <v>9892</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10167</v>
+      </c>
+      <c r="C36" s="2">
+        <v>10167</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4.26</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4.26</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="C41" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="2">
+        <v>11855</v>
+      </c>
+      <c r="C42" s="2">
+        <v>11855</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="2">
+        <v>12564</v>
+      </c>
+      <c r="C43" s="2">
+        <v>12564</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="2">
+        <v>12616</v>
+      </c>
+      <c r="C44" s="2">
+        <v>12616</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="2">
+        <v>12641</v>
+      </c>
+      <c r="C45" s="2">
+        <v>12641</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="2">
+        <v>13704</v>
+      </c>
+      <c r="C46" s="2">
+        <v>13704</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="2">
+        <v>13831</v>
+      </c>
+      <c r="C47" s="2">
+        <v>13831</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="2">
+        <v>13920</v>
+      </c>
+      <c r="C48" s="2">
+        <v>13920</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="2">
+        <v>14533</v>
+      </c>
+      <c r="C49" s="2">
+        <v>14533</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="6">
+        <v>14611</v>
+      </c>
+      <c r="C50" s="6">
+        <v>14611</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="2">
+        <v>14883</v>
+      </c>
+      <c r="C51" s="2">
+        <v>14883</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="6">
+        <v>15784</v>
+      </c>
+      <c r="C54" s="6">
+        <v>15784</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="2">
+        <v>18068</v>
+      </c>
+      <c r="C55" s="2">
+        <v>18068</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="C56" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="2">
+        <v>19488</v>
+      </c>
+      <c r="C57" s="2">
+        <v>19488</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="6">
+        <v>20886</v>
+      </c>
+      <c r="C58" s="6">
+        <v>20886</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="2">
+        <v>21161</v>
+      </c>
+      <c r="C59" s="2">
+        <v>21161</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C62" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="2">
+        <v>3.16</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3.16</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C64" s="2">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="2">
+        <v>5.22</v>
+      </c>
+      <c r="C65" s="2">
+        <v>5.22</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="C66" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="2">
+        <v>24130</v>
+      </c>
+      <c r="C67" s="2">
+        <v>24130</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2.98</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2.98</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="2">
+        <v>6.71</v>
+      </c>
+      <c r="C70" s="2">
+        <v>6.71</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71" s="2">
+        <v>10.32</v>
+      </c>
+      <c r="C71" s="2">
+        <v>10.32</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="2">
+        <v>13.13</v>
+      </c>
+      <c r="C72" s="2">
+        <v>13.13</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" s="2">
+        <v>28398</v>
+      </c>
+      <c r="C73" s="2">
+        <v>28398</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="6">
+        <v>28476</v>
+      </c>
+      <c r="C74" s="6">
+        <v>28476</v>
+      </c>
+      <c r="D74" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2">
+        <v>28747</v>
+      </c>
+      <c r="C75" s="2">
+        <v>28747</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2.37</v>
+      </c>
+      <c r="C78" s="2">
+        <v>2.37</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="C79" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="C80" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2">
+        <v>5.71</v>
+      </c>
+      <c r="C81" s="2">
+        <v>5.71</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="6">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C82" s="6">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2">
+        <v>31854</v>
+      </c>
+      <c r="C83" s="2">
+        <v>31854</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="C86" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="C87" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="C88" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="6">
+        <v>9.94</v>
+      </c>
+      <c r="C89" s="6">
+        <v>9.94</v>
+      </c>
+      <c r="D89" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="2">
+        <v>35077</v>
+      </c>
+      <c r="C90" s="2">
+        <v>35077</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="16"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="16"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="16"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="16"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="16"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="16"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="16"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="16"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="16"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="16"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="16"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="16"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="16"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="16"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="16"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="16"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="16"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="16"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="16"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="16"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="16"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="16"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="16"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="16"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="16"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="16"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="16"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="16"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="16"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="16"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4">
+      <c r="B124" s="4"/>
+      <c r="C124" s="4">
         <v>57254</v>
       </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" ref="D20" si="1">IF(C20&lt;&gt;"",IF(B20&lt;&gt;"",C20-B20,"-"), "-")</f>
+      <c r="D124" s="3" t="str">
+        <f t="shared" ref="D124" si="1">IF(C124&lt;&gt;"",IF(B124&lt;&gt;"",C124-B124,"-"), "-")</f>
         <v>-</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="12" t="s">
+      <c r="E124" s="4"/>
+      <c r="F124" s="3"/>
+    </row>
+    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
+      <c r="B125" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-    </row>
-    <row r="66" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-    </row>
-    <row r="67" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-    </row>
-    <row r="68" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-    </row>
-    <row r="69" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-    </row>
-    <row r="70" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-    </row>
-    <row r="71" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-    </row>
-    <row r="72" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-    </row>
-    <row r="73" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-    </row>
-    <row r="74" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-    </row>
-    <row r="75" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-    </row>
-    <row r="76" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-    </row>
-    <row r="77" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-    </row>
-    <row r="78" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-    </row>
-    <row r="79" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-    </row>
-    <row r="80" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-    </row>
-    <row r="81" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-    </row>
-    <row r="82" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-    </row>
-    <row r="83" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-    </row>
-    <row r="84" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-    </row>
-    <row r="86" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-    </row>
-    <row r="87" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-    </row>
-    <row r="88" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-    </row>
-    <row r="89" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-    </row>
-    <row r="90" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-    </row>
-    <row r="91" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-    </row>
-    <row r="92" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-    </row>
-    <row r="93" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-    </row>
-    <row r="94" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-    </row>
-    <row r="95" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-    </row>
-    <row r="96" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-    </row>
-    <row r="97" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-    </row>
-    <row r="98" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-    </row>
-    <row r="99" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-    </row>
-    <row r="100" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-    </row>
-    <row r="101" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-    </row>
-    <row r="102" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-    </row>
-    <row r="103" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-    </row>
-    <row r="104" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-    </row>
-    <row r="105" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-    </row>
-    <row r="106" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-    </row>
-    <row r="107" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-    </row>
-    <row r="108" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-    </row>
-    <row r="109" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-    </row>
-    <row r="110" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-    </row>
-    <row r="111" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-    </row>
-    <row r="112" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-    </row>
-    <row r="113" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-    </row>
-    <row r="114" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-    </row>
-    <row r="115" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-    </row>
-    <row r="116" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-    </row>
-    <row r="117" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-    </row>
-    <row r="118" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-    </row>
-    <row r="119" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-    </row>
-    <row r="120" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-    </row>
-    <row r="121" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-    </row>
-    <row r="122" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-    </row>
-    <row r="123" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-    </row>
-    <row r="124" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-    </row>
-    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B125" s="4"/>
       <c r="C125" s="4"/>
-    </row>
-    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
-    </row>
-    <row r="127" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
-    </row>
-    <row r="128" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
-    </row>
-    <row r="129" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
-    </row>
-    <row r="130" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
-    </row>
-    <row r="131" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
-    </row>
-    <row r="132" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
-    </row>
-    <row r="133" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
-    </row>
-    <row r="134" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
-    </row>
-    <row r="135" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
-    </row>
-    <row r="136" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
-    </row>
-    <row r="137" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
-    </row>
-    <row r="138" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
-    </row>
-    <row r="139" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
-    </row>
-    <row r="140" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
-    </row>
-    <row r="141" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
-    </row>
-    <row r="142" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
-    </row>
-    <row r="143" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
-    </row>
-    <row r="144" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
-    </row>
-    <row r="145" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
-    </row>
-    <row r="146" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
-    </row>
-    <row r="147" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
-    </row>
-    <row r="148" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
-    </row>
-    <row r="149" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
-    </row>
-    <row r="150" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
-    </row>
-    <row r="151" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
-    </row>
-    <row r="152" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
-    </row>
-    <row r="153" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
-    </row>
-    <row r="154" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
-    </row>
-    <row r="155" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
-    </row>
-    <row r="156" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
-    </row>
-    <row r="157" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
     </row>
@@ -3269,6 +4402,422 @@
     <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
+    </row>
+    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+    </row>
+    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+    </row>
+    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="4"/>
+      <c r="C194" s="4"/>
+    </row>
+    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="4"/>
+      <c r="C195" s="4"/>
+    </row>
+    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="4"/>
+      <c r="C196" s="4"/>
+    </row>
+    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="C197" s="4"/>
+    </row>
+    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="4"/>
+      <c r="C198" s="4"/>
+    </row>
+    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="4"/>
+      <c r="C199" s="4"/>
+    </row>
+    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="4"/>
+      <c r="C200" s="4"/>
+    </row>
+    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="4"/>
+      <c r="C201" s="4"/>
+    </row>
+    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+      <c r="C202" s="4"/>
+    </row>
+    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="4"/>
+      <c r="C203" s="4"/>
+    </row>
+    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="4"/>
+      <c r="C204" s="4"/>
+    </row>
+    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="4"/>
+      <c r="C205" s="4"/>
+    </row>
+    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="4"/>
+      <c r="C206" s="4"/>
+    </row>
+    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="4"/>
+      <c r="C207" s="4"/>
+    </row>
+    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="4"/>
+      <c r="C208" s="4"/>
+    </row>
+    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="4"/>
+      <c r="C209" s="4"/>
+    </row>
+    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="4"/>
+      <c r="C210" s="4"/>
+    </row>
+    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="4"/>
+      <c r="C211" s="4"/>
+    </row>
+    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="4"/>
+      <c r="C212" s="4"/>
+    </row>
+    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="4"/>
+      <c r="C213" s="4"/>
+    </row>
+    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="4"/>
+      <c r="C214" s="4"/>
+    </row>
+    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="4"/>
+      <c r="C215" s="4"/>
+    </row>
+    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="4"/>
+      <c r="C216" s="4"/>
+    </row>
+    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="4"/>
+      <c r="C217" s="4"/>
+    </row>
+    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="4"/>
+      <c r="C218" s="4"/>
+    </row>
+    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="4"/>
+      <c r="C219" s="4"/>
+    </row>
+    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="4"/>
+      <c r="C220" s="4"/>
+    </row>
+    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="4"/>
+      <c r="C221" s="4"/>
+    </row>
+    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="4"/>
+      <c r="C222" s="4"/>
+    </row>
+    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="4"/>
+      <c r="C223" s="4"/>
+    </row>
+    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="4"/>
+      <c r="C224" s="4"/>
+    </row>
+    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="4"/>
+      <c r="C225" s="4"/>
+    </row>
+    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="4"/>
+      <c r="C226" s="4"/>
+    </row>
+    <row r="227" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="4"/>
+      <c r="C227" s="4"/>
+    </row>
+    <row r="228" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="4"/>
+      <c r="C228" s="4"/>
+    </row>
+    <row r="229" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="4"/>
+      <c r="C229" s="4"/>
+    </row>
+    <row r="230" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="4"/>
+      <c r="C230" s="4"/>
+    </row>
+    <row r="231" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="4"/>
+      <c r="C231" s="4"/>
+    </row>
+    <row r="232" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="4"/>
+      <c r="C232" s="4"/>
+    </row>
+    <row r="233" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="4"/>
+      <c r="C233" s="4"/>
+    </row>
+    <row r="234" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="4"/>
+      <c r="C234" s="4"/>
+    </row>
+    <row r="235" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="4"/>
+      <c r="C235" s="4"/>
+    </row>
+    <row r="236" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="4"/>
+      <c r="C236" s="4"/>
+    </row>
+    <row r="237" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="4"/>
+      <c r="C237" s="4"/>
+    </row>
+    <row r="238" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="4"/>
+      <c r="C238" s="4"/>
+    </row>
+    <row r="239" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="4"/>
+      <c r="C239" s="4"/>
+    </row>
+    <row r="240" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="4"/>
+      <c r="C240" s="4"/>
+    </row>
+    <row r="241" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="4"/>
+      <c r="C241" s="4"/>
+    </row>
+    <row r="242" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="4"/>
+      <c r="C242" s="4"/>
+    </row>
+    <row r="243" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="4"/>
+      <c r="C243" s="4"/>
+    </row>
+    <row r="244" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B244" s="4"/>
+      <c r="C244" s="4"/>
+    </row>
+    <row r="245" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B245" s="4"/>
+      <c r="C245" s="4"/>
+    </row>
+    <row r="246" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B246" s="4"/>
+      <c r="C246" s="4"/>
+    </row>
+    <row r="247" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B247" s="4"/>
+      <c r="C247" s="4"/>
+    </row>
+    <row r="248" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B248" s="4"/>
+      <c r="C248" s="4"/>
+    </row>
+    <row r="249" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B249" s="4"/>
+      <c r="C249" s="4"/>
+    </row>
+    <row r="250" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B250" s="4"/>
+      <c r="C250" s="4"/>
+    </row>
+    <row r="251" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B251" s="4"/>
+      <c r="C251" s="4"/>
+    </row>
+    <row r="252" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B252" s="4"/>
+      <c r="C252" s="4"/>
+    </row>
+    <row r="253" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B253" s="4"/>
+      <c r="C253" s="4"/>
+    </row>
+    <row r="254" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B254" s="4"/>
+      <c r="C254" s="4"/>
+    </row>
+    <row r="255" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B255" s="4"/>
+      <c r="C255" s="4"/>
+    </row>
+    <row r="256" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B256" s="4"/>
+      <c r="C256" s="4"/>
+    </row>
+    <row r="257" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B257" s="4"/>
+      <c r="C257" s="4"/>
+    </row>
+    <row r="258" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B258" s="4"/>
+      <c r="C258" s="4"/>
+    </row>
+    <row r="259" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B259" s="4"/>
+      <c r="C259" s="4"/>
+    </row>
+    <row r="260" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B260" s="4"/>
+      <c r="C260" s="4"/>
+    </row>
+    <row r="261" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B261" s="4"/>
+      <c r="C261" s="4"/>
+    </row>
+    <row r="262" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B262" s="4"/>
+      <c r="C262" s="4"/>
+    </row>
+    <row r="263" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B263" s="4"/>
+      <c r="C263" s="4"/>
+    </row>
+    <row r="264" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B264" s="4"/>
+      <c r="C264" s="4"/>
+    </row>
+    <row r="265" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B265" s="4"/>
+      <c r="C265" s="4"/>
+    </row>
+    <row r="266" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B266" s="4"/>
+      <c r="C266" s="4"/>
+    </row>
+    <row r="267" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B267" s="4"/>
+      <c r="C267" s="4"/>
+    </row>
+    <row r="268" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B268" s="4"/>
+      <c r="C268" s="4"/>
+    </row>
+    <row r="269" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B269" s="4"/>
+      <c r="C269" s="4"/>
+    </row>
+    <row r="270" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B270" s="4"/>
+      <c r="C270" s="4"/>
+    </row>
+    <row r="271" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B271" s="4"/>
+      <c r="C271" s="4"/>
+    </row>
+    <row r="272" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B272" s="4"/>
+      <c r="C272" s="4"/>
+    </row>
+    <row r="273" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B273" s="4"/>
+      <c r="C273" s="4"/>
+    </row>
+    <row r="274" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B274" s="4"/>
+      <c r="C274" s="4"/>
+    </row>
+    <row r="275" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B275" s="4"/>
+      <c r="C275" s="4"/>
+    </row>
+    <row r="276" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B276" s="4"/>
+      <c r="C276" s="4"/>
+    </row>
+    <row r="277" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B277" s="4"/>
+      <c r="C277" s="4"/>
+    </row>
+    <row r="278" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B278" s="4"/>
+      <c r="C278" s="4"/>
+    </row>
+    <row r="279" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B279" s="4"/>
+      <c r="C279" s="4"/>
+    </row>
+    <row r="280" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B280" s="4"/>
+      <c r="C280" s="4"/>
+    </row>
+    <row r="281" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B281" s="4"/>
+      <c r="C281" s="4"/>
+    </row>
+    <row r="282" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B282" s="4"/>
+      <c r="C282" s="4"/>
+    </row>
+    <row r="283" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B283" s="4"/>
+      <c r="C283" s="4"/>
+    </row>
+    <row r="284" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B284" s="4"/>
+      <c r="C284" s="4"/>
+    </row>
+    <row r="285" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B285" s="4"/>
+      <c r="C285" s="4"/>
+    </row>
+    <row r="286" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B286" s="4"/>
+      <c r="C286" s="4"/>
+    </row>
+    <row r="287" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B287" s="4"/>
+      <c r="C287" s="4"/>
+    </row>
+    <row r="288" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B288" s="4"/>
+      <c r="C288" s="4"/>
+    </row>
+    <row r="289" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B289" s="4"/>
+      <c r="C289" s="4"/>
+    </row>
+    <row r="290" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B290" s="4"/>
+      <c r="C290" s="4"/>
+    </row>
+    <row r="291" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B291" s="4"/>
+      <c r="C291" s="4"/>
+    </row>
+    <row r="292" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+    </row>
+    <row r="293" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B293" s="4"/>
+      <c r="C293" s="4"/>
+    </row>
+    <row r="294" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B294" s="4"/>
+      <c r="C294" s="4"/>
+    </row>
+    <row r="295" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B295" s="4"/>
+      <c r="C295" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SPO - Mad Clown finished, 9.01 vs 9.05 previous TAS
</commit_message>
<xml_diff>
--- a/SuperPunchout/FrameCompare.xlsx
+++ b/SuperPunchout/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperPunchout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D24D7FA-5BCF-4AC3-ABA6-65DB877AFE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C722511-D348-49A1-9BE6-F34FEFF16A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="5115" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>Place</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>Mad Clown</t>
+  </si>
+  <si>
+    <t>black screen (fight end)</t>
+  </si>
+  <si>
+    <t>Super Macho Man</t>
   </si>
 </sst>
 </file>
@@ -2394,7 +2400,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <selection pane="bottomLeft" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3756,30 +3762,48 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A91" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" s="2">
+        <v>9.01</v>
+      </c>
+      <c r="C91" s="2">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000924E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A92" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="6">
+        <v>37957</v>
+      </c>
+      <c r="C92" s="6">
+        <v>37959</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A93" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93" s="2">
+        <v>38362</v>
+      </c>
+      <c r="C93" s="2">
+        <v>38364</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SPO - up to annoying hard to land punch on Nick Bruiser
</commit_message>
<xml_diff>
--- a/SuperPunchout/FrameCompare.xlsx
+++ b/SuperPunchout/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperPunchout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C722511-D348-49A1-9BE6-F34FEFF16A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B74271-0044-4D44-9DB9-33BE3E3ED500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="5115" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="117">
   <si>
     <t>Place</t>
   </si>
@@ -292,6 +292,96 @@
   </si>
   <si>
     <t>Super Macho Man</t>
+  </si>
+  <si>
+    <t>R stun</t>
+  </si>
+  <si>
+    <t>phase 2 hit 1 (super)</t>
+  </si>
+  <si>
+    <t>Narcis Prince</t>
+  </si>
+  <si>
+    <t>1st punch (gut)</t>
+  </si>
+  <si>
+    <t>2nd punch (gut)</t>
+  </si>
+  <si>
+    <t>3rd punch (guy)</t>
+  </si>
+  <si>
+    <t>4th punch (stun gut)</t>
+  </si>
+  <si>
+    <t>5th punch (delay)</t>
+  </si>
+  <si>
+    <t>back up</t>
+  </si>
+  <si>
+    <t>How Quarlow</t>
+  </si>
+  <si>
+    <t>1st punch (face)</t>
+  </si>
+  <si>
+    <t>2nd punch (face)</t>
+  </si>
+  <si>
+    <t>3rd punch (face)</t>
+  </si>
+  <si>
+    <t>4th punch (gut)</t>
+  </si>
+  <si>
+    <t>Dizzy</t>
+  </si>
+  <si>
+    <t>Gut</t>
+  </si>
+  <si>
+    <t>phase 2 hit 2 (super)</t>
+  </si>
+  <si>
+    <t>Rick Bruiser</t>
+  </si>
+  <si>
+    <t>phase 1 final hit</t>
+  </si>
+  <si>
+    <t>2nd hit (right face stun)</t>
+  </si>
+  <si>
+    <t>4th hit (right gut)</t>
+  </si>
+  <si>
+    <t>5th hit (right face stun)</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2 hit 1 (super)</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Nick Bruiser</t>
+  </si>
+  <si>
+    <t>3rd hit (right face stun)</t>
+  </si>
+  <si>
+    <t>5th hit (right gun delay)</t>
+  </si>
+  <si>
+    <t>6th hit (face)</t>
+  </si>
+  <si>
+    <t>Phase 2 1st hit (super)</t>
   </si>
 </sst>
 </file>
@@ -2396,11 +2486,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
-  <dimension ref="A1:F295"/>
+  <dimension ref="A1:F314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C94" sqref="C94"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2435,7 +2525,7 @@
         <v>190</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D123" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D142" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -3807,409 +3897,743 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="16"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="3" t="str">
+      <c r="A94" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96" s="2">
+        <v>3.94</v>
+      </c>
+      <c r="C96" s="2">
+        <v>3.94</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="C97" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B98" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="C98" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B99" s="2">
+        <v>9.43</v>
+      </c>
+      <c r="C99" s="2">
+        <v>9.43</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="6">
+        <v>42365</v>
+      </c>
+      <c r="C100" s="6">
+        <v>42367</v>
+      </c>
+      <c r="D100" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B101" s="2">
+        <v>42718</v>
+      </c>
+      <c r="C101" s="2">
+        <v>42720</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B104" s="2">
+        <v>1.66</v>
+      </c>
+      <c r="C104" s="2">
+        <v>1.66</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="C105" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B106" s="2">
+        <v>3.77</v>
+      </c>
+      <c r="C106" s="2">
+        <v>3.77</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B107" s="2">
+        <v>4.18</v>
+      </c>
+      <c r="C107" s="2">
+        <v>4.18</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C108" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B109" s="6">
+        <v>45885</v>
+      </c>
+      <c r="C109" s="6">
+        <v>45885</v>
+      </c>
+      <c r="D109" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="2">
+        <v>46287</v>
+      </c>
+      <c r="C110" s="2">
+        <v>46289</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B112" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="C112" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="C113" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2.73</v>
+      </c>
+      <c r="C114" s="2">
+        <v>2.73</v>
+      </c>
+      <c r="D114" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" s="2">
+        <v>4.79</v>
+      </c>
+      <c r="C115" s="2">
+        <v>4.79</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B116" s="2">
+        <v>5.24</v>
+      </c>
+      <c r="C116" s="2">
+        <v>5.24</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" s="2">
+        <v>47022</v>
+      </c>
+      <c r="C117" s="2">
+        <v>47024</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B118" s="2">
+        <v>5.94</v>
+      </c>
+      <c r="C118" s="2">
+        <v>5.94</v>
+      </c>
+      <c r="D118" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B119" s="2">
+        <v>7.45</v>
+      </c>
+      <c r="C119" s="2">
+        <v>7.45</v>
+      </c>
+      <c r="D119" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B120" s="2">
+        <v>8.35</v>
+      </c>
+      <c r="C120" s="2">
+        <v>8.35</v>
+      </c>
+      <c r="D120" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B121" s="6">
+        <v>49273</v>
+      </c>
+      <c r="C121" s="6">
+        <v>49275</v>
+      </c>
+      <c r="D121" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B122" s="2">
+        <v>49660</v>
+      </c>
+      <c r="C122" s="2">
+        <v>49662</v>
+      </c>
+      <c r="D122" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D123" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="C124" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="D124" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B125" s="2">
+        <v>3.03</v>
+      </c>
+      <c r="C125" s="2">
+        <v>3.03</v>
+      </c>
+      <c r="D125" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B126" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="C126" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="D126" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B127" s="2">
+        <v>6.98</v>
+      </c>
+      <c r="C127" s="2">
+        <v>6.98</v>
+      </c>
+      <c r="D127" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B128" s="2">
+        <v>7.64</v>
+      </c>
+      <c r="C128" s="2">
+        <v>7.64</v>
+      </c>
+      <c r="D128" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B129" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="C129" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="D129" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130" s="2">
+        <v>10.65</v>
+      </c>
+      <c r="C130" s="2">
+        <v>10.65</v>
+      </c>
+      <c r="D130" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B131" s="6">
+        <v>52801</v>
+      </c>
+      <c r="C131" s="6">
+        <v>52803</v>
+      </c>
+      <c r="D131" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B132" s="2">
+        <v>53205</v>
+      </c>
+      <c r="C132" s="2">
+        <v>53207</v>
+      </c>
+      <c r="D132" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B133" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="D133" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B134" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="C134" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="D134" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B135" s="2">
+        <v>3.56</v>
+      </c>
+      <c r="C135" s="2">
+        <v>3.56</v>
+      </c>
+      <c r="D135" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B136" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="C136" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D136" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B137" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C137" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="D137" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B138" s="2">
+        <v>5.33</v>
+      </c>
+      <c r="C138" s="2">
+        <v>5.33</v>
+      </c>
+      <c r="D138" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B139" s="2">
+        <v>5.37</v>
+      </c>
+      <c r="C139" s="2">
+        <v>5.37</v>
+      </c>
+      <c r="D139" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2">
+        <v>6.07</v>
+      </c>
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="3" t="str">
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="3" t="str">
-        <f t="shared" si="0"/>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4">
+        <v>57254</v>
+      </c>
+      <c r="D143" s="3" t="str">
+        <f t="shared" ref="D143" si="1">IF(C143&lt;&gt;"",IF(B143&lt;&gt;"",C143-B143,"-"), "-")</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="16"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="16"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="16"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="16"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="16"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="16"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="16"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="16"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="16"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="16"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="16"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="16"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="16"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="16"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="16"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="16"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="16"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="16"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123" s="8"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A124" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4">
-        <v>57254</v>
-      </c>
-      <c r="D124" s="3" t="str">
-        <f t="shared" ref="D124" si="1">IF(C124&lt;&gt;"",IF(B124&lt;&gt;"",C124-B124,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E124" s="4"/>
-      <c r="F124" s="3"/>
-    </row>
-    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
-      <c r="B125" s="12" t="s">
+      <c r="E143" s="4"/>
+      <c r="F143" s="3"/>
+    </row>
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="4"/>
-      <c r="D125" s="3"/>
-    </row>
-    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="3"/>
-    </row>
-    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="3"/>
-    </row>
-    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="3"/>
-    </row>
-    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="3"/>
-    </row>
-    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
-      <c r="B131" s="4"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="3"/>
-    </row>
-    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="3"/>
-    </row>
-    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4"/>
-      <c r="C133" s="4"/>
-      <c r="D133" s="3"/>
-    </row>
-    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="3"/>
-    </row>
-    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="3"/>
-    </row>
-    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="3"/>
-    </row>
-    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
-      <c r="D137" s="3"/>
-    </row>
-    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="3"/>
-    </row>
-    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="3"/>
-    </row>
-    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="3"/>
-    </row>
-    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
-      <c r="D141" s="3"/>
-    </row>
-    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
-      <c r="D142" s="3"/>
-    </row>
-    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="3"/>
     </row>
@@ -4289,145 +4713,183 @@
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
+      <c r="D157" s="3"/>
     </row>
     <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
+      <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
+      <c r="D159" s="3"/>
     </row>
     <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
-    </row>
-    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
-    </row>
-    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
-    </row>
-    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
-    </row>
-    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
-    </row>
-    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
-    </row>
-    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
-    </row>
-    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
-    </row>
-    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
-    </row>
-    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
-    </row>
-    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="4"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
-    </row>
-    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="4"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
-    </row>
-    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="4"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
-    </row>
-    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="4"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
-    </row>
-    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="4"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
-    </row>
-    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
-    </row>
-    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
     </row>
@@ -4842,6 +5304,82 @@
     <row r="295" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B295" s="4"/>
       <c r="C295" s="4"/>
+    </row>
+    <row r="296" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B296" s="4"/>
+      <c r="C296" s="4"/>
+    </row>
+    <row r="297" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B297" s="4"/>
+      <c r="C297" s="4"/>
+    </row>
+    <row r="298" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B298" s="4"/>
+      <c r="C298" s="4"/>
+    </row>
+    <row r="299" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B299" s="4"/>
+      <c r="C299" s="4"/>
+    </row>
+    <row r="300" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B300" s="4"/>
+      <c r="C300" s="4"/>
+    </row>
+    <row r="301" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B301" s="4"/>
+      <c r="C301" s="4"/>
+    </row>
+    <row r="302" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B302" s="4"/>
+      <c r="C302" s="4"/>
+    </row>
+    <row r="303" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B303" s="4"/>
+      <c r="C303" s="4"/>
+    </row>
+    <row r="304" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B304" s="4"/>
+      <c r="C304" s="4"/>
+    </row>
+    <row r="305" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B305" s="4"/>
+      <c r="C305" s="4"/>
+    </row>
+    <row r="306" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B306" s="4"/>
+      <c r="C306" s="4"/>
+    </row>
+    <row r="307" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B307" s="4"/>
+      <c r="C307" s="4"/>
+    </row>
+    <row r="308" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B308" s="4"/>
+      <c r="C308" s="4"/>
+    </row>
+    <row r="309" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B309" s="4"/>
+      <c r="C309" s="4"/>
+    </row>
+    <row r="310" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B310" s="4"/>
+      <c r="C310" s="4"/>
+    </row>
+    <row r="311" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B311" s="4"/>
+      <c r="C311" s="4"/>
+    </row>
+    <row r="312" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B312" s="4"/>
+      <c r="C312" s="4"/>
+    </row>
+    <row r="313" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B313" s="4"/>
+      <c r="C313" s="4"/>
+    </row>
+    <row r="314" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B314" s="4"/>
+      <c r="C314" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SPO - v6 done, 28 realtime frames saved, no clock time savings
</commit_message>
<xml_diff>
--- a/SuperPunchout/FrameCompare.xlsx
+++ b/SuperPunchout/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperPunchout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54771A4C-69F0-49BA-885D-0F4FC6F0B32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BA33F9-F92D-4A23-9461-DBFC83ABAE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42780" yWindow="630" windowWidth="15375" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="102">
   <si>
     <t>Place</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t>V6</t>
+  </si>
+  <si>
+    <t>4th punch (face delay)</t>
+  </si>
+  <si>
+    <t>5th punch (left face counter)</t>
+  </si>
+  <si>
+    <t>"1"</t>
+  </si>
+  <si>
+    <t>3rd punch (gut)</t>
   </si>
 </sst>
 </file>
@@ -799,11 +811,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7E52CC-3356-4254-B5E7-E1B0B655F38D}">
-  <dimension ref="A1:F317"/>
+  <dimension ref="A1:F321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -838,7 +850,7 @@
         <v>190</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D145" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D149" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -1575,39 +1587,45 @@
       <c r="A52" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="2">
+        <v>14855</v>
+      </c>
       <c r="C52" s="2">
         <v>14883</v>
       </c>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D52" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="2">
+        <v>0.24</v>
+      </c>
       <c r="C53" s="2">
         <v>0.24</v>
       </c>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="2">
+        <v>2.3199999999999998</v>
+      </c>
       <c r="C54" s="2">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1627,26 +1645,30 @@
       <c r="A56" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="2">
+        <v>18040</v>
+      </c>
       <c r="C56" s="2">
         <v>18068</v>
       </c>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>3.52</v>
+      </c>
       <c r="C57" s="2">
         <v>3.52</v>
       </c>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1679,182 +1701,210 @@
       <c r="A60" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="2">
+        <v>21133</v>
+      </c>
       <c r="C60" s="2">
         <v>21161</v>
       </c>
-      <c r="D60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="2">
+        <v>0.26</v>
+      </c>
       <c r="C61" s="2">
         <v>0.26</v>
       </c>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D61" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="2">
+        <v>1.64</v>
+      </c>
       <c r="C62" s="2">
         <v>1.64</v>
       </c>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D62" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="2">
+        <v>2.3199999999999998</v>
+      </c>
       <c r="C63" s="2">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D63" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B64" s="2"/>
+      <c r="B64" s="2">
+        <v>3.16</v>
+      </c>
       <c r="C64" s="2">
         <v>3.16</v>
       </c>
-      <c r="D64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D64" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="2"/>
+      <c r="B65" s="2">
+        <v>4.5599999999999996</v>
+      </c>
       <c r="C65" s="2">
         <v>4.5599999999999996</v>
       </c>
-      <c r="D65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D65" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="2"/>
+      <c r="B66" s="2">
+        <v>5.22</v>
+      </c>
       <c r="C66" s="2">
         <v>5.22</v>
       </c>
-      <c r="D66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D66" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="5"/>
+      <c r="B67" s="5">
+        <v>6.3</v>
+      </c>
       <c r="C67" s="5">
         <v>6.3</v>
       </c>
-      <c r="D67" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D67" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="2">
+        <v>24102</v>
+      </c>
       <c r="C68" s="2">
         <v>24130</v>
       </c>
-      <c r="D68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D68" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B69" s="2"/>
+      <c r="B69" s="2">
+        <v>0.24</v>
+      </c>
       <c r="C69" s="2">
         <v>0.24</v>
       </c>
-      <c r="D69" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D69" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="2"/>
+      <c r="B70" s="2">
+        <v>2.98</v>
+      </c>
       <c r="C70" s="2">
         <v>2.98</v>
       </c>
-      <c r="D70" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D70" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="2"/>
+      <c r="B71" s="2">
+        <v>6.71</v>
+      </c>
       <c r="C71" s="2">
         <v>6.71</v>
       </c>
-      <c r="D71" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D71" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="2"/>
+      <c r="B72" s="2">
+        <v>10.32</v>
+      </c>
       <c r="C72" s="2">
         <v>10.32</v>
       </c>
-      <c r="D72" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D72" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="2"/>
+      <c r="B73" s="2">
+        <v>13.13</v>
+      </c>
       <c r="C73" s="2">
         <v>13.13</v>
       </c>
-      <c r="D73" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D73" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1887,959 +1937,1127 @@
       <c r="A76" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="2"/>
+      <c r="B76" s="2">
+        <v>28719</v>
+      </c>
       <c r="C76" s="2">
         <v>28747</v>
       </c>
-      <c r="D76" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D76" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B77" s="2"/>
+      <c r="B77" s="2">
+        <v>0.26</v>
+      </c>
       <c r="C77" s="2">
         <v>0.26</v>
       </c>
-      <c r="D77" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D77" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="2"/>
+      <c r="B78" s="2">
+        <v>1.67</v>
+      </c>
       <c r="C78" s="2">
         <v>1.67</v>
       </c>
-      <c r="D78" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D78" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="2"/>
+      <c r="B79" s="2">
+        <v>2.37</v>
+      </c>
       <c r="C79" s="2">
         <v>2.37</v>
       </c>
-      <c r="D79" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D79" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B80" s="2"/>
+      <c r="B80" s="2">
+        <v>3.32</v>
+      </c>
       <c r="C80" s="2">
         <v>3.32</v>
       </c>
-      <c r="D80" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D80" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B81" s="2"/>
+      <c r="B81" s="2">
+        <v>5.15</v>
+      </c>
       <c r="C81" s="2">
         <v>5.15</v>
       </c>
-      <c r="D81" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D81" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B82" s="2"/>
+      <c r="B82" s="2">
+        <v>5.71</v>
+      </c>
       <c r="C82" s="2">
         <v>5.71</v>
       </c>
-      <c r="D82" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D82" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="5"/>
+      <c r="B83" s="5">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="C83" s="5">
         <v>8.4499999999999993</v>
       </c>
-      <c r="D83" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D83" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B84" s="2"/>
+      <c r="B84" s="11">
+        <v>31826</v>
+      </c>
       <c r="C84" s="2">
         <v>31854</v>
       </c>
-      <c r="D84" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D84" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B85" s="2"/>
+      <c r="B85" s="2">
+        <v>0.3</v>
+      </c>
       <c r="C85" s="2">
         <v>0.3</v>
       </c>
-      <c r="D85" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D85" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B86" s="2"/>
+      <c r="B86" s="2">
+        <v>1.75</v>
+      </c>
       <c r="C86" s="2">
         <v>1.75</v>
       </c>
-      <c r="D86" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D86" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B87" s="2"/>
+      <c r="B87" s="2">
+        <v>4.07</v>
+      </c>
       <c r="C87" s="2">
         <v>4.07</v>
       </c>
-      <c r="D87" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D87" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B88" s="2"/>
+      <c r="B88" s="2">
+        <v>5.99</v>
+      </c>
       <c r="C88" s="2">
         <v>5.99</v>
       </c>
-      <c r="D88" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D88" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B89" s="2"/>
+      <c r="B89" s="2">
+        <v>6.03</v>
+      </c>
       <c r="C89" s="2">
         <v>6.03</v>
       </c>
-      <c r="D89" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D89" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B90" s="5"/>
+      <c r="B90" s="5">
+        <v>9.94</v>
+      </c>
       <c r="C90" s="5">
         <v>9.94</v>
       </c>
-      <c r="D90" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D90" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B91" s="2"/>
+      <c r="B91" s="2">
+        <v>35049</v>
+      </c>
       <c r="C91" s="2">
         <v>35077</v>
       </c>
-      <c r="D91" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D91" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B92" s="2"/>
+      <c r="A92" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1.77</v>
+      </c>
       <c r="C92" s="2">
-        <v>9.01</v>
-      </c>
-      <c r="D92" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1.77</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5">
-        <v>37957</v>
-      </c>
-      <c r="D93" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A93" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" s="2">
+        <v>2.94</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2.94</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" s="2"/>
+      <c r="A94" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="2">
+        <v>3.64</v>
+      </c>
       <c r="C94" s="2">
-        <v>38362</v>
-      </c>
-      <c r="D94" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3.64</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B95" s="2"/>
+      <c r="A95" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="2">
+        <v>36081</v>
+      </c>
       <c r="C95" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="D95" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>36109</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B96" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B96" s="2">
+        <v>9.01</v>
+      </c>
       <c r="C96" s="2">
-        <v>1.67</v>
-      </c>
-      <c r="D96" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>9.01</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2">
-        <v>3.94</v>
-      </c>
-      <c r="D97" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A97" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97" s="5">
+        <v>37929</v>
+      </c>
+      <c r="C97" s="5">
+        <v>37957</v>
+      </c>
+      <c r="D97" s="6">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B98" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B98" s="2">
+        <v>38334</v>
+      </c>
       <c r="C98" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="D98" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>38362</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B99" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.24</v>
+      </c>
       <c r="C99" s="2">
-        <v>7.13</v>
-      </c>
-      <c r="D99" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.24</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B100" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B100" s="2">
+        <v>1.67</v>
+      </c>
       <c r="C100" s="2">
-        <v>9.43</v>
-      </c>
-      <c r="D100" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1.67</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5">
-        <v>42365</v>
-      </c>
-      <c r="D101" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A101" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B101" s="2">
+        <v>3.94</v>
+      </c>
+      <c r="C101" s="2">
+        <v>3.94</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B102" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B102" s="2">
+        <v>6.5</v>
+      </c>
       <c r="C102" s="2">
-        <v>42718</v>
-      </c>
-      <c r="D102" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>6.5</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B103" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="B103" s="2">
+        <v>7.13</v>
+      </c>
       <c r="C103" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="D103" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>7.13</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B104" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B104" s="2">
+        <v>9.43</v>
+      </c>
       <c r="C104" s="2">
-        <v>0.96</v>
-      </c>
-      <c r="D104" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>9.43</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2">
-        <v>1.66</v>
-      </c>
-      <c r="D105" s="3" t="str">
+      <c r="A105" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5">
+        <v>42365</v>
+      </c>
+      <c r="D105" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B106" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="B106" s="2">
+        <v>42690</v>
+      </c>
       <c r="C106" s="2">
-        <v>2.52</v>
-      </c>
-      <c r="D106" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>42718</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B107" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="B107" s="2">
+        <v>0.26</v>
+      </c>
       <c r="C107" s="2">
-        <v>3.77</v>
-      </c>
-      <c r="D107" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.26</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B108" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="B108" s="2">
+        <v>0.96</v>
+      </c>
       <c r="C108" s="2">
-        <v>4.18</v>
-      </c>
-      <c r="D108" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.96</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="2"/>
+      <c r="A109" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B109" s="2">
+        <v>1.66</v>
+      </c>
       <c r="C109" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D109" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1.66</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5">
-        <v>45885</v>
-      </c>
-      <c r="D110" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A110" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="C110" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B111" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="B111" s="2">
+        <v>3.77</v>
+      </c>
       <c r="C111" s="2">
-        <v>46287</v>
-      </c>
-      <c r="D111" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3.77</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B112" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="B112" s="2">
+        <v>4.18</v>
+      </c>
       <c r="C112" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="D112" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4.18</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B113" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B113" s="2">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="C113" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="D113" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="D114" s="3" t="str">
+      <c r="A114" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5">
+        <v>45885</v>
+      </c>
+      <c r="D114" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B115" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B115" s="2">
+        <v>46259</v>
+      </c>
       <c r="C115" s="2">
-        <v>2.73</v>
-      </c>
-      <c r="D115" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>46287</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B116" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="B116" s="2">
+        <v>0.24</v>
+      </c>
       <c r="C116" s="2">
-        <v>4.79</v>
-      </c>
-      <c r="D116" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.24</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B117" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.92</v>
+      </c>
       <c r="C117" s="2">
-        <v>5.24</v>
-      </c>
-      <c r="D117" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.92</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B118" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="B118" s="2">
+        <v>2.0299999999999998</v>
+      </c>
       <c r="C118" s="2">
-        <v>47022</v>
-      </c>
-      <c r="D118" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D118" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B119" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="B119" s="2">
+        <v>2.73</v>
+      </c>
       <c r="C119" s="2">
-        <v>5.94</v>
-      </c>
-      <c r="D119" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2.73</v>
+      </c>
+      <c r="D119" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B120" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="B120" s="2">
+        <v>4.79</v>
+      </c>
       <c r="C120" s="2">
-        <v>7.45</v>
-      </c>
-      <c r="D120" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4.79</v>
+      </c>
+      <c r="D120" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B121" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="B121" s="2">
+        <v>5.24</v>
+      </c>
       <c r="C121" s="2">
-        <v>8.35</v>
-      </c>
-      <c r="D121" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>5.24</v>
+      </c>
+      <c r="D121" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5">
-        <v>49273</v>
-      </c>
-      <c r="D122" s="6" t="str">
+      <c r="A122" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2">
+        <v>47022</v>
+      </c>
+      <c r="D122" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B123" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="B123" s="2">
+        <v>5.94</v>
+      </c>
       <c r="C123" s="2">
-        <v>49660</v>
-      </c>
-      <c r="D123" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>5.94</v>
+      </c>
+      <c r="D123" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B124" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="B124" s="2">
+        <v>7.45</v>
+      </c>
       <c r="C124" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="D124" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>7.45</v>
+      </c>
+      <c r="D124" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B125" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B125" s="2">
+        <v>8.35</v>
+      </c>
       <c r="C125" s="2">
-        <v>1.64</v>
-      </c>
-      <c r="D125" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>8.35</v>
+      </c>
+      <c r="D125" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2">
-        <v>3.03</v>
-      </c>
-      <c r="D126" s="3" t="str">
+      <c r="A126" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5">
+        <v>49273</v>
+      </c>
+      <c r="D126" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B127" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="B127" s="2">
+        <v>49632</v>
+      </c>
       <c r="C127" s="2">
-        <v>3.9</v>
-      </c>
-      <c r="D127" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>49660</v>
+      </c>
+      <c r="D127" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B128" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B128" s="2">
+        <v>0.24</v>
+      </c>
       <c r="C128" s="2">
-        <v>6.98</v>
-      </c>
-      <c r="D128" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.24</v>
+      </c>
+      <c r="D128" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B129" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="B129" s="2">
+        <v>1.64</v>
+      </c>
       <c r="C129" s="2">
-        <v>7.64</v>
-      </c>
-      <c r="D129" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1.64</v>
+      </c>
+      <c r="D129" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B130" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B130" s="2">
+        <v>3.03</v>
+      </c>
       <c r="C130" s="2">
-        <v>9.99</v>
-      </c>
-      <c r="D130" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3.03</v>
+      </c>
+      <c r="D130" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B131" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B131" s="2">
+        <v>3.9</v>
+      </c>
       <c r="C131" s="2">
-        <v>10.65</v>
-      </c>
-      <c r="D131" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3.9</v>
+      </c>
+      <c r="D131" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B132" s="5"/>
-      <c r="C132" s="5">
-        <v>52801</v>
-      </c>
-      <c r="D132" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A132" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B132" s="2">
+        <v>6.98</v>
+      </c>
+      <c r="C132" s="2">
+        <v>6.98</v>
+      </c>
+      <c r="D132" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B133" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B133" s="2">
+        <v>7.64</v>
+      </c>
       <c r="C133" s="2">
-        <v>53205</v>
-      </c>
-      <c r="D133" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>7.64</v>
+      </c>
+      <c r="D133" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B134" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B134" s="2">
+        <v>9.99</v>
+      </c>
       <c r="C134" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="D134" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>9.99</v>
+      </c>
+      <c r="D134" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B135" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B135" s="2">
+        <v>10.65</v>
+      </c>
       <c r="C135" s="2">
-        <v>1.94</v>
-      </c>
-      <c r="D135" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>10.65</v>
+      </c>
+      <c r="D135" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2">
-        <v>3.56</v>
-      </c>
-      <c r="D136" s="3" t="str">
+      <c r="A136" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5">
+        <v>52801</v>
+      </c>
+      <c r="D136" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B137" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="B137" s="2">
+        <v>53177</v>
+      </c>
       <c r="C137" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="D137" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>53205</v>
+      </c>
+      <c r="D137" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B138" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B138" s="2">
+        <v>0.22</v>
+      </c>
       <c r="C138" s="2">
-        <v>4.88</v>
-      </c>
-      <c r="D138" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>0.22</v>
+      </c>
+      <c r="D138" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B139" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B139" s="2">
+        <v>1.94</v>
+      </c>
       <c r="C139" s="2">
-        <v>5.33</v>
-      </c>
-      <c r="D139" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1.94</v>
+      </c>
+      <c r="D139" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B140" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="B140" s="2">
+        <v>3.56</v>
+      </c>
       <c r="C140" s="2">
-        <v>5.37</v>
-      </c>
-      <c r="D140" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3.56</v>
+      </c>
+      <c r="D140" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B141" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="B141" s="2">
+        <v>4.2</v>
+      </c>
       <c r="C141" s="2">
-        <v>6.07</v>
-      </c>
-      <c r="D141" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4.2</v>
+      </c>
+      <c r="D141" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B142" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B142" s="2">
+        <v>4.88</v>
+      </c>
       <c r="C142" s="2">
-        <v>8.52</v>
-      </c>
-      <c r="D142" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4.88</v>
+      </c>
+      <c r="D142" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B143" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B143" s="2">
+        <v>5.33</v>
+      </c>
       <c r="C143" s="2">
-        <v>56455</v>
-      </c>
-      <c r="D143" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>5.33</v>
+      </c>
+      <c r="D143" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B144" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="B144" s="2">
+        <v>5.37</v>
+      </c>
       <c r="C144" s="2">
-        <v>56582</v>
-      </c>
-      <c r="D144" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>5.37</v>
+      </c>
+      <c r="D144" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B145" s="2">
+        <v>6.07</v>
+      </c>
+      <c r="C145" s="2">
+        <v>6.07</v>
+      </c>
+      <c r="D145" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" s="2">
+        <v>8.52</v>
+      </c>
+      <c r="C146" s="2">
+        <v>8.52</v>
+      </c>
+      <c r="D146" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B147" s="2">
+        <v>56427</v>
+      </c>
+      <c r="C147" s="2">
+        <v>56455</v>
+      </c>
+      <c r="D147" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B148" s="2">
+        <v>56554</v>
+      </c>
+      <c r="C148" s="2">
+        <v>56582</v>
+      </c>
+      <c r="D148" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2">
+      <c r="B149" s="2">
+        <v>56643</v>
+      </c>
+      <c r="C149" s="2">
         <v>56671</v>
       </c>
-      <c r="D145" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146" s="7" t="s">
+      <c r="D149" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="4"/>
-      <c r="C146" s="4">
+      <c r="B150" s="4">
+        <v>57224</v>
+      </c>
+      <c r="C150" s="4">
         <v>57252</v>
       </c>
-      <c r="D146" s="3" t="str">
-        <f t="shared" ref="D146" si="1">IF(C146&lt;&gt;"",IF(B146&lt;&gt;"",C146-B146,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E146" s="4"/>
-      <c r="F146" s="3"/>
-    </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A147" s="4"/>
-      <c r="B147" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D147" s="3"/>
-    </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148" s="4"/>
-      <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="3"/>
-    </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="3"/>
-    </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="3"/>
+      <c r="D150" s="3">
+        <f t="shared" ref="D150" si="1">IF(C150&lt;&gt;"",IF(B150&lt;&gt;"",C150-B150,"-"), "-")</f>
+        <v>28</v>
+      </c>
+      <c r="E150" s="4"/>
+      <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="B151" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -3008,25 +3226,33 @@
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
+      <c r="D179" s="3"/>
     </row>
     <row r="180" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
+      <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
+      <c r="D181" s="3"/>
     </row>
     <row r="182" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
     </row>
     <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
     </row>
@@ -3561,6 +3787,22 @@
     <row r="317" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B317" s="4"/>
       <c r="C317" s="4"/>
+    </row>
+    <row r="318" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B318" s="4"/>
+      <c r="C318" s="4"/>
+    </row>
+    <row r="319" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B319" s="4"/>
+      <c r="C319" s="4"/>
+    </row>
+    <row r="320" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B320" s="4"/>
+      <c r="C320" s="4"/>
+    </row>
+    <row r="321" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B321" s="4"/>
+      <c r="C321" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>